<commit_message>
completed dataset including 4 years of stats, and created static version of plot to build shiny app off of
</commit_message>
<xml_diff>
--- a/DF/334FinalProjData.xlsx
+++ b/DF/334FinalProjData.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benlestage/Desktop/ds334_final_project/DF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15653F31-63ED-3546-A5D9-CFBBE2D140B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DE120F-5414-1E40-B8C3-9D95A4D947AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="27420" windowHeight="16940"/>
+    <workbookView xWindow="1000" yWindow="500" windowWidth="27420" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="334FinalProjData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -106,7 +119,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -940,106 +953,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
@@ -1049,40 +1064,43 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A27">
+    <sortCondition ref="A1:A27"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>